<commit_message>
Aerobic scope model selection
</commit_message>
<xml_diff>
--- a/results/AS results/gamm_AS_model_selection.xlsx
+++ b/results/AS results/gamm_AS_model_selection.xlsx
@@ -50,22 +50,22 @@
     <t xml:space="preserve">m20</t>
   </si>
   <si>
+    <t xml:space="preserve">aerobic_scope ~ s(doy, by = fish_basin, bs = "cc", k = 17) + s(floy_tag, year, by = fish_basin, bs = c("re", "re"), k = c(20, 4)) + ACF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aerobic_scope ~ fish_basin + s(doy, by = fish_basin, bs = "cc", k = 17) + s(floy_tag, year, by = fish_basin, bs = c("re", "re"), k = c(20, 4)) + ACF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m19</t>
+  </si>
+  <si>
     <t xml:space="preserve">aerobic_scope ~ fish_basin + s(doy, by = fish_basin, bs = "cc", k = 17) + s(floy_tag, year, by = fish_basin, bs = c("re", "re"), k = c(20, 4)) + ti(doy, fish_basin, bs = c("cc", "fs"), k = c(20, 3))</t>
   </si>
   <si>
     <t xml:space="preserve">m8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aerobic_scope ~ fish_basin + s(doy, by = fish_basin, bs = "cc", k = 17) + s(floy_tag, year, by = fish_basin, bs = c("re", "re"), k = c(20, 4)) + ACF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">m19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aerobic_scope ~ s(doy, by = fish_basin, bs = "cc", k = 17) + s(floy_tag, year, by = fish_basin, bs = c("re", "re"), k = c(20, 4)) + ACF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">m21</t>
   </si>
   <si>
     <t xml:space="preserve">aerobic_scope ~ s(doy, by = fish_basin, bs = "cc", k = 17) + s(floy_tag, year, by = fish_basin, bs = c("re", "re"), k = c(20, 4))</t>
@@ -512,28 +512,28 @@
         <v>11</v>
       </c>
       <c r="C2" t="n">
-        <v>77.137203835238</v>
+        <v>75.3940389498535</v>
       </c>
       <c r="D2" t="n">
-        <v>-66992.1351366059</v>
+        <v>-66613.2146299122</v>
       </c>
       <c r="E2" t="n">
-        <v>134142.197058439</v>
+        <v>133381.131621427</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>0.999999772843637</v>
+        <v>1</v>
       </c>
       <c r="H2" t="n">
-        <v>134751.498648707</v>
+        <v>133977.992975931</v>
       </c>
       <c r="I2" t="n">
-        <v>395.965513102236</v>
+        <v>401.054344111106</v>
       </c>
       <c r="J2" t="n">
-        <v>16507.8627961648</v>
+        <v>16509.6059610501</v>
       </c>
     </row>
     <row r="3">
@@ -544,28 +544,28 @@
         <v>13</v>
       </c>
       <c r="C3" t="n">
-        <v>77.4466570389077</v>
+        <v>62.7084781667592</v>
       </c>
       <c r="D3" t="n">
-        <v>-67007.1455135324</v>
+        <v>-66762.0660903263</v>
       </c>
       <c r="E3" t="n">
-        <v>134172.792312448</v>
+        <v>133652.438076203</v>
       </c>
       <c r="F3" t="n">
-        <v>30.5952540096769</v>
+        <v>271.306454775709</v>
       </c>
       <c r="G3" t="n">
-        <v>0.000000227156363184419</v>
+        <v>0.0000000000000000000000000000000000000000000000000000000000122053965217866</v>
       </c>
       <c r="H3" t="n">
-        <v>134784.310397268</v>
+        <v>134147.458512967</v>
       </c>
       <c r="I3" t="n">
-        <v>395.702420303694</v>
+        <v>408.780894170596</v>
       </c>
       <c r="J3" t="n">
-        <v>16507.5533429611</v>
+        <v>16522.2915218332</v>
       </c>
     </row>
     <row r="4">
@@ -576,28 +576,28 @@
         <v>15</v>
       </c>
       <c r="C4" t="n">
-        <v>63.0075497832943</v>
+        <v>62.7241569845925</v>
       </c>
       <c r="D4" t="n">
-        <v>-67168.2896186385</v>
+        <v>-66762.1072299664</v>
       </c>
       <c r="E4" t="n">
-        <v>134465.294526559</v>
+        <v>133652.548544725</v>
       </c>
       <c r="F4" t="n">
-        <v>323.097468120046</v>
+        <v>271.416923298122</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0000000000000000000000000000000000000000000000000000000000000000000000692271002723184</v>
+        <v>0.0000000000000000000000000000000000000000000000000000000000115495206111892</v>
       </c>
       <c r="H4" t="n">
-        <v>134961.894456321</v>
+        <v>134147.677739164</v>
       </c>
       <c r="I4" t="n">
-        <v>404.467418401191</v>
+        <v>408.78049079072</v>
       </c>
       <c r="J4" t="n">
-        <v>16521.9924502167</v>
+        <v>16522.2758430154</v>
       </c>
     </row>
     <row r="5">
@@ -608,28 +608,28 @@
         <v>17</v>
       </c>
       <c r="C5" t="n">
-        <v>62.9927649547946</v>
+        <v>77.4466570389077</v>
       </c>
       <c r="D5" t="n">
-        <v>-67168.3236111186</v>
+        <v>-67007.1455135324</v>
       </c>
       <c r="E5" t="n">
-        <v>134465.336702528</v>
+        <v>134172.792312448</v>
       </c>
       <c r="F5" t="n">
-        <v>323.139644088835</v>
+        <v>791.660691021068</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0000000000000000000000000000000000000000000000000000000000000000000000677825253819906</v>
+        <v>0.0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001238982507667</v>
       </c>
       <c r="H5" t="n">
-        <v>134961.837057923</v>
+        <v>134784.310397268</v>
       </c>
       <c r="I5" t="n">
-        <v>404.4670207527</v>
+        <v>395.702420303694</v>
       </c>
       <c r="J5" t="n">
-        <v>16522.0072350452</v>
+        <v>16507.5533429611</v>
       </c>
     </row>
     <row r="6">
@@ -649,10 +649,10 @@
         <v>134502.394285043</v>
       </c>
       <c r="F6" t="n">
-        <v>360.197226604621</v>
+        <v>1121.26266361601</v>
       </c>
       <c r="G6" t="n">
-        <v>0.000000000000000000000000000000000000000000000000000000000000000000000000000000608367416590225</v>
+        <v>3.31822792381082e-244</v>
       </c>
       <c r="H6" t="n">
         <v>134999.040295596</v>
@@ -681,10 +681,10 @@
         <v>134502.409673592</v>
       </c>
       <c r="F7" t="n">
-        <v>360.212615153345</v>
+        <v>1121.27805216474</v>
       </c>
       <c r="G7" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000060370443291687</v>
+        <v>3.29279453896598e-244</v>
       </c>
       <c r="H7" t="n">
         <v>134999.131566702</v>
@@ -713,7 +713,7 @@
         <v>135823.962373645</v>
       </c>
       <c r="F8" t="n">
-        <v>1681.76531520617</v>
+        <v>2442.83075221756</v>
       </c>
       <c r="G8" t="n">
         <v>0</v>
@@ -745,7 +745,7 @@
         <v>141953.545415288</v>
       </c>
       <c r="F9" t="n">
-        <v>7811.34835684969</v>
+        <v>8572.41379386108</v>
       </c>
       <c r="G9" t="n">
         <v>0</v>
@@ -777,7 +777,7 @@
         <v>141968.597180972</v>
       </c>
       <c r="F10" t="n">
-        <v>7826.40012253303</v>
+        <v>8587.46555954442</v>
       </c>
       <c r="G10" t="n">
         <v>0</v>
@@ -809,7 +809,7 @@
         <v>141968.992872762</v>
       </c>
       <c r="F11" t="n">
-        <v>7826.79581432327</v>
+        <v>8587.86125133466</v>
       </c>
       <c r="G11" t="n">
         <v>0</v>
@@ -841,7 +841,7 @@
         <v>142037.870884761</v>
       </c>
       <c r="F12" t="n">
-        <v>7895.67382632231</v>
+        <v>8656.7392633337</v>
       </c>
       <c r="G12" t="n">
         <v>0</v>
@@ -873,7 +873,7 @@
         <v>142121.030804876</v>
       </c>
       <c r="F13" t="n">
-        <v>7978.83374643771</v>
+        <v>8739.8991834491</v>
       </c>
       <c r="G13" t="n">
         <v>0</v>
@@ -905,7 +905,7 @@
         <v>142137.034205063</v>
       </c>
       <c r="F14" t="n">
-        <v>7994.83714662446</v>
+        <v>8755.90258363585</v>
       </c>
       <c r="G14" t="n">
         <v>0</v>
@@ -937,7 +937,7 @@
         <v>142884.163945898</v>
       </c>
       <c r="F15" t="n">
-        <v>8741.96688745965</v>
+        <v>9503.03232447105</v>
       </c>
       <c r="G15" t="n">
         <v>0</v>
@@ -969,7 +969,7 @@
         <v>142884.163945898</v>
       </c>
       <c r="F16" t="n">
-        <v>8741.96688745965</v>
+        <v>9503.03232447105</v>
       </c>
       <c r="G16" t="n">
         <v>0</v>
@@ -1001,7 +1001,7 @@
         <v>153938.210179625</v>
       </c>
       <c r="F17" t="n">
-        <v>19796.013121186</v>
+        <v>20557.0785581974</v>
       </c>
       <c r="G17" t="n">
         <v>0</v>
@@ -1033,7 +1033,7 @@
         <v>157400.37203466</v>
       </c>
       <c r="F18" t="n">
-        <v>23258.1749762211</v>
+        <v>24019.2404132324</v>
       </c>
       <c r="G18" t="n">
         <v>0</v>

</xml_diff>